<commit_message>
update fouling and coral protocols
</commit_message>
<xml_diff>
--- a/fouling/final_spreadsheets/fouling_community_data_entry_spreadsheet_marinegeo.xlsx
+++ b/fouling/final_spreadsheets/fouling_community_data_entry_spreadsheet_marinegeo.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>definition</t>
   </si>
@@ -116,6 +116,24 @@
   </si>
   <si>
     <t xml:space="preserve">sample metadata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deployment_latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panel deployment latitude in decimal degrees, to five decimal places</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xx.xxxxx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deployment_longitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panel deployment longitude in decimal degrees, to five decimal places</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xxx.xxxxx</t>
   </si>
   <si>
     <t xml:space="preserve">identification_notes</t>
@@ -946,36 +964,40 @@
         <v>25</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>27</v>
+      </c>
       <c r="E8" s="10"/>
       <c r="F8" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="E9" s="10"/>
       <c r="F9" s="10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>12</v>
@@ -986,43 +1008,39 @@
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>33</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="10" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>36</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13">
@@ -1051,104 +1069,108 @@
         <v>41</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10" t="s">
-        <v>18</v>
-      </c>
+      <c r="D15" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="10"/>
       <c r="F15" s="10" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="10" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D16" s="10"/>
-      <c r="E16" s="10" t="s">
-        <v>18</v>
-      </c>
+      <c r="E16" s="10"/>
       <c r="F16" s="10" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="10" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
+      <c r="E17" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="F17" s="10" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="10" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
+      <c r="E18" s="10" t="s">
+        <v>18</v>
+      </c>
       <c r="F18" s="10" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>13</v>
@@ -1156,67 +1178,63 @@
       <c r="D20" s="10"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="10" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>33</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D22" s="10"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="10" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>36</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D23" s="10"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>17</v>
@@ -1226,66 +1244,102 @@
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="10" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="E25" s="10"/>
       <c r="F25" s="10" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="10"/>
+        <v>17</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>45</v>
+      </c>
       <c r="E26" s="10"/>
       <c r="F26" s="10" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="10" t="s">
-        <v>69</v>
-      </c>
+      <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
+      <c r="A28" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1326,43 +1380,51 @@
     <col min="7" max="7" width="21.71" hidden="0" customWidth="1"/>
     <col min="8" max="8" width="22.71" hidden="0" customWidth="1"/>
     <col min="9" max="9" width="20.71" hidden="0" customWidth="1"/>
-    <col min="10" max="10" width="14.71" hidden="0" customWidth="1"/>
-    <col min="11" max="11" width="21.71" hidden="0" customWidth="1"/>
+    <col min="10" max="10" width="19.71" hidden="0" customWidth="1"/>
+    <col min="11" max="11" width="20.71" hidden="0" customWidth="1"/>
+    <col min="12" max="12" width="14.71" hidden="0" customWidth="1"/>
+    <col min="13" max="13" width="21.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>61</v>
-      </c>
       <c r="H1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="12" t="s">
         <v>59</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1394,34 +1456,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>61</v>
-      </c>
       <c r="E1" s="12" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>15</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="K1" s="12" t="s">
         <v>11</v>
@@ -1456,37 +1518,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>55</v>
-      </c>
       <c r="J1" s="12" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1519,40 +1581,40 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>61</v>
-      </c>
       <c r="E1" s="12" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="I1" s="12" t="s">
         <v>19</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1585,40 +1647,40 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>55</v>
-      </c>
       <c r="K1" s="12" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="L1" s="12" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>